<commit_message>
v1.3.4 fix english dictionary
</commit_message>
<xml_diff>
--- a/ai/assets/textbook/pinyin/chat_important.xlsx
+++ b/ai/assets/textbook/pinyin/chat_important.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\AIChatFilter\service\ai-chatfilter-service\ai\assets\textbook\pinyin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD66D27-3D6B-4FAB-8627-658F26B44743}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0104EE-6161-4786-A7DF-82D8E2E0593C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1035" yWindow="2835" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -494,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
v1.3.6 fix tcpsocket bug for error log and allow some symbol can pass in prefilter
</commit_message>
<xml_diff>
--- a/ai/assets/textbook/pinyin/chat_important.xlsx
+++ b/ai/assets/textbook/pinyin/chat_important.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\AIChatFilter\service\ai-chatfilter-service\ai\assets\textbook\pinyin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0104EE-6161-4786-A7DF-82D8E2E0593C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F807C1-B83E-416E-B6E2-6474C5CD8145}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1035" yWindow="2835" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>发言内容</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -154,6 +154,25 @@
   </si>
   <si>
     <t>其实赢不难，?{65}关住公棕呺</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>并音</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>并音   多有力气</t>
+  </si>
+  <si>
+    <t>语文幷</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>拼音就能联续到我</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>并音就能联续到我</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -492,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -752,6 +771,46 @@
         <v>1</v>
       </c>
     </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:B4" xr:uid="{D5E2A364-7B88-4106-9A95-3E56C3C6E261}"/>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
v1.3.6 hotfix for 1.3.5
</commit_message>
<xml_diff>
--- a/ai/assets/textbook/pinyin/chat_important.xlsx
+++ b/ai/assets/textbook/pinyin/chat_important.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\AIChatFilter\service\ai-chatfilter-service\ai\assets\textbook\pinyin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F807C1-B83E-416E-B6E2-6474C5CD8145}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6DFC7DE-0784-42E6-8BF8-CBC22914DF7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1035" yWindow="2835" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4095" yWindow="2640" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>发言内容</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -173,6 +173,46 @@
   </si>
   <si>
     <t>并音就能联续到我</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>公棕呺</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>公棕呺 大神探路</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>关注工众号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>关注公棕呺</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>叉叉695叉叉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>叉叉511叉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>叉511叉叉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>叉65叉45</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>叉叉396叉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>叉65叉45叉</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -511,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -811,6 +851,86 @@
         <v>1</v>
       </c>
     </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>44</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:B4" xr:uid="{D5E2A364-7B88-4106-9A95-3E56C3C6E261}"/>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
v1.3.6 add textbook english and chinese change prefilter for english allowed sentence add freq system in split word
</commit_message>
<xml_diff>
--- a/ai/assets/textbook/pinyin/chat_important.xlsx
+++ b/ai/assets/textbook/pinyin/chat_important.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\AIChatFilter\service\ai-chatfilter-service\ai\assets\textbook\pinyin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6DFC7DE-0784-42E6-8BF8-CBC22914DF7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F0665F-E7E5-4721-BDEC-F3F8DE3F007E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4095" yWindow="2640" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="2985" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>发言内容</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -214,13 +214,21 @@
   <si>
     <t>叉65叉45叉</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>工众号</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>并音工众号</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,6 +249,12 @@
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
     </font>
   </fonts>
   <fills count="2">
@@ -551,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -931,6 +945,22 @@
         <v>1</v>
       </c>
     </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:B4" xr:uid="{D5E2A364-7B88-4106-9A95-3E56C3C6E261}"/>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>